<commit_message>
Clean up autarky and multi
</commit_message>
<xml_diff>
--- a/tables/createClosed.xlsx
+++ b/tables/createClosed.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7461" uniqueCount="4610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8083" uniqueCount="4996">
   <si>
     <t>Row</t>
   </si>
@@ -13822,6 +13822,1164 @@
   </si>
   <si>
     <t>Labor Force</t>
+  </si>
+  <si>
+    <t>S/S Population, Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>S/S Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>S/S Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Autoregression in Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Autoregression in Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>Autoregression in Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ref_ch</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>ih</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>netw</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>pih</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>py3</t>
+  </si>
+  <si>
+    <t>py2</t>
+  </si>
+  <si>
+    <t>py1</t>
+  </si>
+  <si>
+    <t>py0</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>pq</t>
+  </si>
+  <si>
+    <t>ngdp</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>puk</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w0</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rbl</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>roc_py</t>
+  </si>
+  <si>
+    <t>ref_roc_py</t>
+  </si>
+  <si>
+    <t>roc_w</t>
+  </si>
+  <si>
+    <t>roc_pch</t>
+  </si>
+  <si>
+    <t>roc_ih</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>roc_k</t>
+  </si>
+  <si>
+    <t>ych</t>
+  </si>
+  <si>
+    <t>ycg</t>
+  </si>
+  <si>
+    <t>yih</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>pcg</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>txl1</t>
+  </si>
+  <si>
+    <t>txl2</t>
+  </si>
+  <si>
+    <t>roc_cg</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>gg_a</t>
+  </si>
+  <si>
+    <t>gg_nn</t>
+  </si>
+  <si>
+    <t>shk_ar</t>
+  </si>
+  <si>
+    <t>shk_r</t>
+  </si>
+  <si>
+    <t>shk_w</t>
+  </si>
+  <si>
+    <t>shk_curr</t>
+  </si>
+  <si>
+    <t>shk_cg</t>
+  </si>
+  <si>
+    <t>shk_txl1</t>
+  </si>
+  <si>
+    <t>shk_txl2</t>
+  </si>
+  <si>
+    <t>shk_nr</t>
+  </si>
+  <si>
+    <t>shk_nw_to_nn</t>
+  </si>
+  <si>
+    <t>shk_nf_to_nw</t>
+  </si>
+  <si>
+    <t>gg_shk_a</t>
+  </si>
+  <si>
+    <t>gg_shk_nn</t>
+  </si>
+  <si>
+    <t>rho_ar</t>
+  </si>
+  <si>
+    <t>chi_curr</t>
+  </si>
+  <si>
+    <t>chi_ch</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>nu_0</t>
+  </si>
+  <si>
+    <t>nu_1</t>
+  </si>
+  <si>
+    <t>xi_k</t>
+  </si>
+  <si>
+    <t>xi_ih</t>
+  </si>
+  <si>
+    <t>upsilon_0</t>
+  </si>
+  <si>
+    <t>upsilon_1</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta_k</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_n0</t>
+  </si>
+  <si>
+    <t>gamma_n</t>
+  </si>
+  <si>
+    <t>gamma_uk</t>
+  </si>
+  <si>
+    <t>gamma_q</t>
+  </si>
+  <si>
+    <t>gamma_z</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>kappa_1</t>
+  </si>
+  <si>
+    <t>kappa_2</t>
+  </si>
+  <si>
+    <t>ss_ar</t>
+  </si>
+  <si>
+    <t>ss_roc_pch</t>
+  </si>
+  <si>
+    <t>xi_py</t>
+  </si>
+  <si>
+    <t>mu_py</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>psi_pch</t>
+  </si>
+  <si>
+    <t>mu_y3</t>
+  </si>
+  <si>
+    <t>zeta_py</t>
+  </si>
+  <si>
+    <t>xi_ch0</t>
+  </si>
+  <si>
+    <t>xi_ch1</t>
+  </si>
+  <si>
+    <t>xi_ch2</t>
+  </si>
+  <si>
+    <t>xi_y2</t>
+  </si>
+  <si>
+    <t>xi_y1</t>
+  </si>
+  <si>
+    <t>ss_dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>ss_ncg_to_ngdp</t>
+  </si>
+  <si>
+    <t>tau_cg</t>
+  </si>
+  <si>
+    <t>tau_txl1</t>
+  </si>
+  <si>
+    <t>rho_cg</t>
+  </si>
+  <si>
+    <t>rho_txl2</t>
+  </si>
+  <si>
+    <t>rho_txl1</t>
+  </si>
+  <si>
+    <t>ss_nr</t>
+  </si>
+  <si>
+    <t>ss_nw_to_nn</t>
+  </si>
+  <si>
+    <t>ss_nf_to_nw</t>
+  </si>
+  <si>
+    <t>rho_nr</t>
+  </si>
+  <si>
+    <t>rho_nw</t>
+  </si>
+  <si>
+    <t>rho_nf</t>
+  </si>
+  <si>
+    <t>gg_rho_a</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_a</t>
+  </si>
+  <si>
+    <t>gg_rho_nn</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_nn</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Real Discount Factor</t>
+  </si>
+  <si>
+    <t>Private Consumption</t>
+  </si>
+  <si>
+    <t>Private Consumption, Point of Reference</t>
+  </si>
+  <si>
+    <t>Per-Capita Labor Supply</t>
+  </si>
+  <si>
+    <t>Variable Labor</t>
+  </si>
+  <si>
+    <t>Private Investment</t>
+  </si>
+  <si>
+    <t>Production Capital</t>
+  </si>
+  <si>
+    <t>Production Capital, Point of Reference</t>
+  </si>
+  <si>
+    <t>Production Capital Services</t>
+  </si>
+  <si>
+    <t>Household Net Worth</t>
+  </si>
+  <si>
+    <t>Domestic Technology Level</t>
+  </si>
+  <si>
+    <t>Shadow Value of Household Budget Constraing</t>
+  </si>
+  <si>
+    <t>Price of Private Consumption</t>
+  </si>
+  <si>
+    <t>Price of Private Investment</t>
+  </si>
+  <si>
+    <t>Domestic Intermediate Inputs</t>
+  </si>
+  <si>
+    <t>Stage T-3 Output</t>
+  </si>
+  <si>
+    <t>Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Stage T-1 Output</t>
+  </si>
+  <si>
+    <t>Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-3 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-2 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-1 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Commodity Input into Production</t>
+  </si>
+  <si>
+    <t>Price of Commodity Input into Production</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Price of Domestic Production</t>
+  </si>
+  <si>
+    <t>Price of Production Capital</t>
+  </si>
+  <si>
+    <t>Price of Production Capital Services</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Money Market Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Household Lending Rate</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change, Point of Reference</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Consumer Goods, Rate of Change</t>
+  </si>
+  <si>
+    <t>Household Investment, Rate of Change</t>
+  </si>
+  <si>
+    <t>Capital Utilization Rate</t>
+  </si>
+  <si>
+    <t>Household Capital, Rate of Change</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Government Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Investment</t>
+  </si>
+  <si>
+    <t>Government Debt Interest Rate</t>
+  </si>
+  <si>
+    <t>Price of Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Debt to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Wealthy Consumers</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Poor Consumers</t>
+  </si>
+  <si>
+    <t>Government Consumption, Rate of Change</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Working Age Population</t>
+  </si>
+  <si>
+    <t>Labor Force</t>
+  </si>
+  <si>
+    <t>Markup to Cover Overhead Labor</t>
+  </si>
+  <si>
+    <t>S/S Population, Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>S/S Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>S/S Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Autoregression in Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Autoregression in Share of Working Age Population in Total Population</t>
+  </si>
+  <si>
+    <t>Autoregression in Labor Participation Rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>ref_ch</t>
+  </si>
+  <si>
+    <t>nh</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>ih</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>netw</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>pih</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>py3</t>
+  </si>
+  <si>
+    <t>py2</t>
+  </si>
+  <si>
+    <t>py1</t>
+  </si>
+  <si>
+    <t>py0</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>pq</t>
+  </si>
+  <si>
+    <t>ngdp</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>puk</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w0</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rbl</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>roc_py</t>
+  </si>
+  <si>
+    <t>ref_roc_py</t>
+  </si>
+  <si>
+    <t>roc_w</t>
+  </si>
+  <si>
+    <t>roc_pch</t>
+  </si>
+  <si>
+    <t>roc_ih</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>roc_k</t>
+  </si>
+  <si>
+    <t>ych</t>
+  </si>
+  <si>
+    <t>ycg</t>
+  </si>
+  <si>
+    <t>yih</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>pcg</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>txl1</t>
+  </si>
+  <si>
+    <t>txl2</t>
+  </si>
+  <si>
+    <t>roc_cg</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>gg_a</t>
+  </si>
+  <si>
+    <t>gg_nn</t>
+  </si>
+  <si>
+    <t>shk_ar</t>
+  </si>
+  <si>
+    <t>shk_r</t>
+  </si>
+  <si>
+    <t>shk_w</t>
+  </si>
+  <si>
+    <t>shk_curr</t>
+  </si>
+  <si>
+    <t>shk_cg</t>
+  </si>
+  <si>
+    <t>shk_txl1</t>
+  </si>
+  <si>
+    <t>shk_txl2</t>
+  </si>
+  <si>
+    <t>shk_nr</t>
+  </si>
+  <si>
+    <t>shk_nw_to_nn</t>
+  </si>
+  <si>
+    <t>shk_nf_to_nw</t>
+  </si>
+  <si>
+    <t>gg_shk_a</t>
+  </si>
+  <si>
+    <t>gg_shk_nn</t>
+  </si>
+  <si>
+    <t>rho_ar</t>
+  </si>
+  <si>
+    <t>chi_curr</t>
+  </si>
+  <si>
+    <t>chi_ch</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>nu_0</t>
+  </si>
+  <si>
+    <t>nu_1</t>
+  </si>
+  <si>
+    <t>xi_k</t>
+  </si>
+  <si>
+    <t>xi_ih</t>
+  </si>
+  <si>
+    <t>upsilon_0</t>
+  </si>
+  <si>
+    <t>upsilon_1</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta_k</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_n0</t>
+  </si>
+  <si>
+    <t>gamma_n</t>
+  </si>
+  <si>
+    <t>gamma_uk</t>
+  </si>
+  <si>
+    <t>gamma_q</t>
+  </si>
+  <si>
+    <t>gamma_z</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>rho_w</t>
+  </si>
+  <si>
+    <t>kappa_1</t>
+  </si>
+  <si>
+    <t>kappa_2</t>
+  </si>
+  <si>
+    <t>ss_ar</t>
+  </si>
+  <si>
+    <t>ss_roc_pch</t>
+  </si>
+  <si>
+    <t>xi_py</t>
+  </si>
+  <si>
+    <t>mu_py</t>
+  </si>
+  <si>
+    <t>rho_r</t>
+  </si>
+  <si>
+    <t>psi_pch</t>
+  </si>
+  <si>
+    <t>mu_y3</t>
+  </si>
+  <si>
+    <t>zeta_py</t>
+  </si>
+  <si>
+    <t>xi_ch0</t>
+  </si>
+  <si>
+    <t>xi_ch1</t>
+  </si>
+  <si>
+    <t>xi_ch2</t>
+  </si>
+  <si>
+    <t>xi_y2</t>
+  </si>
+  <si>
+    <t>xi_y1</t>
+  </si>
+  <si>
+    <t>ss_dg_to_ngdp</t>
+  </si>
+  <si>
+    <t>ss_ncg_to_ngdp</t>
+  </si>
+  <si>
+    <t>tau_cg</t>
+  </si>
+  <si>
+    <t>tau_txl1</t>
+  </si>
+  <si>
+    <t>rho_cg</t>
+  </si>
+  <si>
+    <t>rho_txl2</t>
+  </si>
+  <si>
+    <t>rho_txl1</t>
+  </si>
+  <si>
+    <t>ss_nr</t>
+  </si>
+  <si>
+    <t>ss_nw_to_nn</t>
+  </si>
+  <si>
+    <t>ss_nf_to_nw</t>
+  </si>
+  <si>
+    <t>rho_nr</t>
+  </si>
+  <si>
+    <t>rho_nw</t>
+  </si>
+  <si>
+    <t>rho_nf</t>
+  </si>
+  <si>
+    <t>gg_rho_a</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_a</t>
+  </si>
+  <si>
+    <t>gg_rho_nn</t>
+  </si>
+  <si>
+    <t>gg_ss_roc_nn</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff-</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Real Discount Factor</t>
+  </si>
+  <si>
+    <t>Private Consumption</t>
+  </si>
+  <si>
+    <t>Private Consumption, Point of Reference</t>
+  </si>
+  <si>
+    <t>Per-Capita Labor Supply</t>
+  </si>
+  <si>
+    <t>Variable Labor</t>
+  </si>
+  <si>
+    <t>Private Investment</t>
+  </si>
+  <si>
+    <t>Production Capital</t>
+  </si>
+  <si>
+    <t>Production Capital, Point of Reference</t>
+  </si>
+  <si>
+    <t>Production Capital Services</t>
+  </si>
+  <si>
+    <t>Household Net Worth</t>
+  </si>
+  <si>
+    <t>Domestic Technology Level</t>
+  </si>
+  <si>
+    <t>Shadow Value of Household Budget Constraing</t>
+  </si>
+  <si>
+    <t>Price of Private Consumption</t>
+  </si>
+  <si>
+    <t>Price of Private Investment</t>
+  </si>
+  <si>
+    <t>Domestic Intermediate Inputs</t>
+  </si>
+  <si>
+    <t>Stage T-3 Output</t>
+  </si>
+  <si>
+    <t>Stage T-2 Output</t>
+  </si>
+  <si>
+    <t>Stage T-1 Output</t>
+  </si>
+  <si>
+    <t>Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-3 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-2 Output</t>
+  </si>
+  <si>
+    <t>Price of State T-1 Output</t>
+  </si>
+  <si>
+    <t>Price of Stage T-0 Output</t>
+  </si>
+  <si>
+    <t>Commodity Input into Production</t>
+  </si>
+  <si>
+    <t>Price of Commodity Input into Production</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Price of Domestic Production</t>
+  </si>
+  <si>
+    <t>Price of Production Capital</t>
+  </si>
+  <si>
+    <t>Price of Production Capital Services</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Money Market Rate</t>
+  </si>
+  <si>
+    <t>Nominal Local Currency Household Lending Rate</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Final Domestic Output, Rate of Change, Point of Reference</t>
+  </si>
+  <si>
+    <t>Nominal Wage Rate, Rate of Change</t>
+  </si>
+  <si>
+    <t>Price of Consumer Goods, Rate of Change</t>
+  </si>
+  <si>
+    <t>Household Investment, Rate of Change</t>
+  </si>
+  <si>
+    <t>Capital Utilization Rate</t>
+  </si>
+  <si>
+    <t>Household Capital, Rate of Change</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Government Consumption</t>
+  </si>
+  <si>
+    <t>Domestic Component of Private Investment</t>
+  </si>
+  <si>
+    <t>Government Debt Interest Rate</t>
+  </si>
+  <si>
+    <t>Price of Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Consumption</t>
+  </si>
+  <si>
+    <t>Government Debt to GDP Ratio</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Wealthy Consumers</t>
+  </si>
+  <si>
+    <t>Net Lump-Sum Tax Rate on Poor Consumers</t>
+  </si>
+  <si>
+    <t>Government Consumption, Rate of Change</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Total Population Relative to Global Population Component</t>
+  </si>
+  <si>
+    <t>Working Age Population</t>
+  </si>
+  <si>
+    <t>Labor Force</t>
+  </si>
+  <si>
+    <t>Markup to Cover Overhead Labor</t>
   </si>
   <si>
     <t>S/S Population, Relative to Global Population Component</t>
@@ -13863,7 +15021,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -13895,11 +15053,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -13925,6 +15085,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13934,7 +15096,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E123"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="true"/>
@@ -13949,194 +15111,194 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>4426</v>
+        <v>4803</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4545</v>
+        <v>4926</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4546</v>
+        <v>4927</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4547</v>
+        <v>4928</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4552</v>
+        <v>4933</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>4427</v>
+        <v>4804</v>
       </c>
       <c r="B2" s="0">
-        <v>0.93137254901960842</v>
+        <v>0.93137254901960764</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>4553</v>
+        <v>4934</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>4428</v>
+        <v>4805</v>
       </c>
       <c r="B3" s="0">
-        <v>0.60528213526869767</v>
+        <v>0.61501661590482737</v>
       </c>
       <c r="C3" s="0">
-        <v>1.0301999999999996</v>
+        <v>1.0302</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>4554</v>
+        <v>4935</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>4429</v>
+        <v>4806</v>
       </c>
       <c r="B4" s="0">
-        <v>0.14399999999999996</v>
+        <v>0.10523076923076924</v>
       </c>
       <c r="C4" s="0">
-        <v>1.0301999999999993</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>4555</v>
+        <v>4936</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4430</v>
+        <v>4807</v>
       </c>
       <c r="B5" s="0">
-        <v>2.4276080020926898</v>
+        <v>1.7459420310423139</v>
       </c>
       <c r="C5" s="0">
         <v>0.99999999999999967</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>4556</v>
+        <v>4937</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>4431</v>
+        <v>4808</v>
       </c>
       <c r="B6" s="0">
-        <v>0.7930186140169454</v>
+        <v>0.57034106347382252</v>
       </c>
       <c r="C6" s="0">
-        <v>1.0099999999999996</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>4557</v>
+        <v>4938</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>4432</v>
+        <v>4809</v>
       </c>
       <c r="B7" s="0">
-        <v>0.19471786473130229</v>
+        <v>0.18498338409517256</v>
       </c>
       <c r="C7" s="0">
-        <v>1.0301999999999987</v>
+        <v>1.0301999999999991</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>4558</v>
+        <v>4939</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>4433</v>
+        <v>4810</v>
       </c>
       <c r="B8" s="0">
-        <v>1.1131983587468848</v>
+        <v>1.057546516619573</v>
       </c>
       <c r="C8" s="0">
-        <v>1.0301999999999987</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>4559</v>
+        <v>4940</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>4434</v>
+        <v>4811</v>
       </c>
       <c r="B9" s="0">
-        <v>1.113198358746885</v>
+        <v>1.057546516619573</v>
       </c>
       <c r="C9" s="0">
-        <v>1.0301999999999985</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>4560</v>
+        <v>4941</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>4435</v>
+        <v>4812</v>
       </c>
       <c r="B10" s="0">
-        <v>1.113198358746885</v>
+        <v>1.0575465166195728</v>
       </c>
       <c r="C10" s="0">
-        <v>1.0301999999999987</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>4561</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>4436</v>
+        <v>4813</v>
       </c>
       <c r="B11" s="0">
-        <v>0.0066085189309093729</v>
+        <v>0.0068608444985979473</v>
       </c>
       <c r="C11" s="0">
-        <v>0.97068530382448714</v>
+        <v>0.97068530382450047</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>4562</v>
+        <v>4943</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>4437</v>
+        <v>4814</v>
       </c>
       <c r="B12" s="0">
         <v>1</v>
@@ -14145,32 +15307,32 @@
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>4563</v>
+        <v>4944</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>4438</v>
+        <v>4815</v>
       </c>
       <c r="B13" s="0">
-        <v>1.6521221125353034</v>
+        <v>1.6259723300788802</v>
       </c>
       <c r="C13" s="0">
-        <v>0.97068530382450058</v>
+        <v>0.97068530382450013</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>4564</v>
+        <v>4945</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>4439</v>
+        <v>4816</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
@@ -14179,749 +15341,757 @@
         <v>1.01</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>4565</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>4440</v>
+        <v>4817</v>
       </c>
       <c r="B15" s="0">
         <v>1</v>
       </c>
       <c r="C15" s="0">
-        <v>1.0100000000000002</v>
+        <v>1.01</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>4566</v>
+        <v>4947</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>4441</v>
+        <v>4818</v>
       </c>
       <c r="B16" s="0">
         <v>1.1999999999999997</v>
       </c>
       <c r="C16" s="0">
-        <v>1.0301999999999991</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>4567</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>4442</v>
+        <v>4819</v>
       </c>
       <c r="B17" s="0">
-        <v>3.4646238961310503</v>
+        <v>4.5821322046472774</v>
       </c>
       <c r="C17" s="0">
         <v>1.0301999999999998</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>4568</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>4443</v>
+        <v>4820</v>
       </c>
       <c r="B18" s="0">
-        <v>2.2000000000000002</v>
+        <v>2.5489443914406191</v>
       </c>
       <c r="C18" s="0">
-        <v>1.0301999999999993</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>4569</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>4444</v>
+        <v>4821</v>
       </c>
       <c r="B19" s="0">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C19" s="0">
-        <v>1.0301999999999993</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>4570</v>
+        <v>4951</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>4445</v>
+        <v>4822</v>
       </c>
       <c r="B20" s="0">
-        <v>0.90909090909090917</v>
+        <v>1</v>
       </c>
       <c r="C20" s="0">
-        <v>1.01</v>
+        <v>1.0302</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>4571</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>4446</v>
+        <v>4823</v>
       </c>
       <c r="B21" s="0">
-        <v>0.36363636363636365</v>
+        <v>0.09951698895494912</v>
       </c>
       <c r="C21" s="0">
         <v>1.01</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>4572</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>4447</v>
+        <v>4824</v>
       </c>
       <c r="B22" s="0">
-        <v>0.13854317651506606</v>
+        <v>0.29816264432919271</v>
       </c>
       <c r="C22" s="0">
-        <v>1.0099999999999996</v>
+        <v>1.01</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>4573</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>4448</v>
+        <v>4825</v>
       </c>
       <c r="B23" s="0">
-        <v>1</v>
+        <v>0.36363636363636359</v>
       </c>
       <c r="C23" s="0">
-        <v>1.0405019999999994</v>
+        <v>1.01</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>4574</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>4449</v>
+        <v>4826</v>
       </c>
       <c r="B24" s="0">
-        <v>1</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="C24" s="0">
         <v>1.01</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>4575</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>4450</v>
+        <v>4827</v>
       </c>
       <c r="B25" s="0">
-        <v>1</v>
+        <v>0.13415496797055887</v>
       </c>
       <c r="C25" s="0">
-        <v>1.01</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>4576</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>4451</v>
+        <v>4828</v>
       </c>
       <c r="B26" s="0">
-        <v>0.28745999981550496</v>
+        <v>0.29816264432919271</v>
       </c>
       <c r="C26" s="0">
-        <v>1.0100000000000002</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>4577</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>4452</v>
+        <v>4829</v>
       </c>
       <c r="B27" s="0">
-        <v>0.60528213526869779</v>
+        <v>1</v>
       </c>
       <c r="C27" s="0">
-        <v>1.0301999999999996</v>
+        <v>1.0405019999999998</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>4578</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>4453</v>
+        <v>4830</v>
       </c>
       <c r="B28" s="0">
-        <v>0.60528213526869767</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0">
-        <v>1.0301999999999996</v>
+        <v>1.01</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>4548</v>
-      </c>
-      <c r="E28" s="0"/>
+        <v>4929</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>4960</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>4454</v>
+        <v>4831</v>
       </c>
       <c r="B29" s="0">
-        <v>1.0843776755894032</v>
+        <v>1</v>
       </c>
       <c r="C29" s="0">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>4579</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>4455</v>
+        <v>4832</v>
       </c>
       <c r="B30" s="0">
-        <v>1.0843776755894035</v>
+        <v>0.2874578046663423</v>
       </c>
       <c r="C30" s="0">
-        <v>1</v>
+        <v>1.0100000000000002</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>4580</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>4456</v>
+        <v>4833</v>
       </c>
       <c r="B31" s="0">
-        <v>0.45565991793734434</v>
+        <v>0.61501661590482748</v>
       </c>
       <c r="C31" s="0">
-        <v>1.0405019999999994</v>
+        <v>1.0302</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>4581</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>4457</v>
+        <v>4834</v>
       </c>
       <c r="B32" s="0">
-        <v>1.01</v>
+        <v>0.61501661590482748</v>
       </c>
       <c r="C32" s="0">
-        <v>1.0000000000000002</v>
+        <v>1.0302</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>4548</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>4582</v>
-      </c>
+        <v>4929</v>
+      </c>
+      <c r="E32" s="0"/>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>4458</v>
+        <v>4835</v>
       </c>
       <c r="B33" s="0">
-        <v>1.0099999999999998</v>
+        <v>1.0843752951234378</v>
       </c>
       <c r="C33" s="0">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>4583</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>4459</v>
+        <v>4836</v>
       </c>
       <c r="B34" s="0">
-        <v>1.0301999999999996</v>
+        <v>1.0843752951234378</v>
       </c>
       <c r="C34" s="0">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>4584</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>4460</v>
+        <v>4837</v>
       </c>
       <c r="B35" s="0">
-        <v>1.0100000000000002</v>
+        <v>0.45287732583097862</v>
       </c>
       <c r="C35" s="0">
-        <v>1</v>
+        <v>1.0405019999999998</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>4585</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>4461</v>
+        <v>4838</v>
       </c>
       <c r="B36" s="0">
-        <v>1.0301999999999989</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="C36" s="0">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>4586</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>4462</v>
+        <v>4839</v>
       </c>
       <c r="B37" s="0">
-        <v>1</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="C37" s="0">
         <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>4587</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>4463</v>
+        <v>4840</v>
       </c>
       <c r="B38" s="0">
-        <v>1.0301999999999987</v>
+        <v>1.0302</v>
       </c>
       <c r="C38" s="0">
         <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>4588</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>4464</v>
+        <v>4841</v>
       </c>
       <c r="B39" s="0">
-        <v>0.60528213526869779</v>
+        <v>1.01</v>
       </c>
       <c r="C39" s="0">
-        <v>1.0301999999999996</v>
+        <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>4589</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>4465</v>
+        <v>4842</v>
       </c>
       <c r="B40" s="0">
-        <v>0.20000000000000001</v>
+        <v>1.0301999999999991</v>
       </c>
       <c r="C40" s="0">
-        <v>1.0301999999999993</v>
+        <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>4590</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>4466</v>
+        <v>4843</v>
       </c>
       <c r="B41" s="0">
-        <v>0.19471786473130229</v>
+        <v>1</v>
       </c>
       <c r="C41" s="0">
-        <v>1.0301999999999989</v>
+        <v>1</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>4591</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>4467</v>
+        <v>4844</v>
       </c>
       <c r="B42" s="0">
-        <v>1.0843776755894032</v>
+        <v>1.0301999999999996</v>
       </c>
       <c r="C42" s="0">
         <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>4592</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>4468</v>
+        <v>4845</v>
       </c>
       <c r="B43" s="0">
-        <v>1</v>
+        <v>0.61501661590482737</v>
       </c>
       <c r="C43" s="0">
-        <v>1.01</v>
+        <v>1.0302</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>4593</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>4469</v>
+        <v>4846</v>
       </c>
       <c r="B44" s="0">
         <v>0.20000000000000001</v>
       </c>
       <c r="C44" s="0">
-        <v>1.0301999999999993</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>4548</v>
+        <v>4929</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>4594</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>4470</v>
+        <v>4847</v>
       </c>
       <c r="B45" s="0">
-        <v>0.40000000000000002</v>
+        <v>0.18498338409517256</v>
       </c>
       <c r="C45" s="0">
-        <v>-4.7472244854295966e-18</v>
+        <v>1.0301999999999993</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>4549</v>
+        <v>4929</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>4595</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>4471</v>
+        <v>4848</v>
       </c>
       <c r="B46" s="0">
-        <v>0.35829096148293182</v>
+        <v>1.0843752951234378</v>
       </c>
       <c r="C46" s="0">
-        <v>-1.1119165676337587e-16</v>
+        <v>1</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>4549</v>
+        <v>4929</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>4596</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>4472</v>
+        <v>4849</v>
       </c>
       <c r="B47" s="0">
-        <v>1.1200528622635776e-27</v>
+        <v>1</v>
       </c>
       <c r="C47" s="0">
-        <v>-3.5017833481733839e-28</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>4549</v>
+        <v>4929</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>4597</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>4473</v>
+        <v>4850</v>
       </c>
       <c r="B48" s="0">
-        <v>1.0301999999999993</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C48" s="0">
-        <v>1</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>4550</v>
+        <v>4929</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>4598</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>4474</v>
+        <v>4851</v>
       </c>
       <c r="B49" s="0">
-        <v>1</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C49" s="0">
-        <v>1.0099999999999998</v>
+        <v>8.4685489933965657e-19</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>4550</v>
+        <v>4930</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>4599</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>4475</v>
+        <v>4852</v>
       </c>
       <c r="B50" s="0">
-        <v>1</v>
+        <v>0.35261844555645727</v>
       </c>
       <c r="C50" s="0">
-        <v>1</v>
+        <v>-1.7234735811879524e-17</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>4550</v>
+        <v>4930</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>4600</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>4476</v>
+        <v>4853</v>
       </c>
       <c r="B51" s="0">
-        <v>0.69999999999999996</v>
+        <v>5.2313643640623786e-30</v>
       </c>
       <c r="C51" s="0">
-        <v>1.01</v>
+        <v>-1.9967513716726523e-30</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>4550</v>
+        <v>4930</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>4601</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>4477</v>
+        <v>4854</v>
       </c>
       <c r="B52" s="0">
-        <v>0.48999999999999994</v>
+        <v>1.0301999999999998</v>
       </c>
       <c r="C52" s="0">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>4550</v>
+        <v>4931</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>4602</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>4478</v>
+        <v>4855</v>
       </c>
       <c r="B53" s="0">
-        <v>4.3689061453190767</v>
+        <v>1</v>
       </c>
       <c r="C53" s="0">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>4550</v>
-      </c>
-      <c r="E53" s="0"/>
+        <v>4931</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>4984</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>4479</v>
+        <v>4856</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
       </c>
       <c r="C54" s="0">
-        <v>1.0100000000000002</v>
+        <v>1</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>4550</v>
-      </c>
-      <c r="E54" s="0"/>
+        <v>4931</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>4985</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>4480</v>
+        <v>4857</v>
       </c>
       <c r="B55" s="0">
-        <v>0</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>0</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E55" s="0"/>
+        <v>4931</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>4986</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>4481</v>
+        <v>4858</v>
       </c>
       <c r="B56" s="0">
-        <v>0</v>
+        <v>0.48999999999999994</v>
       </c>
       <c r="C56" s="0">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E56" s="0"/>
+        <v>4931</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>4987</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>4482</v>
+        <v>4859</v>
       </c>
       <c r="B57" s="0">
-        <v>0</v>
+        <v>8.034021216600669</v>
       </c>
       <c r="C57" s="0">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>4551</v>
+        <v>4931</v>
       </c>
       <c r="E57" s="0"/>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>4483</v>
+        <v>4860</v>
       </c>
       <c r="B58" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="0">
-        <v>0</v>
+        <v>1.0099999999999998</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>4551</v>
+        <v>4931</v>
       </c>
       <c r="E58" s="0"/>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>4484</v>
+        <v>4861</v>
       </c>
       <c r="B59" s="0">
         <v>0</v>
@@ -14930,13 +16100,13 @@
         <v>0</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E59" s="0"/>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>4485</v>
+        <v>4862</v>
       </c>
       <c r="B60" s="0">
         <v>0</v>
@@ -14945,13 +16115,13 @@
         <v>0</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E60" s="0"/>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>4486</v>
+        <v>4863</v>
       </c>
       <c r="B61" s="0">
         <v>0</v>
@@ -14960,13 +16130,13 @@
         <v>0</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E61" s="0"/>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>4487</v>
+        <v>4864</v>
       </c>
       <c r="B62" s="0">
         <v>0</v>
@@ -14975,13 +16145,13 @@
         <v>0</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E62" s="0"/>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>4488</v>
+        <v>4865</v>
       </c>
       <c r="B63" s="0">
         <v>0</v>
@@ -14990,13 +16160,13 @@
         <v>0</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>4489</v>
+        <v>4866</v>
       </c>
       <c r="B64" s="0">
         <v>0</v>
@@ -15005,13 +16175,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E64" s="0"/>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>4490</v>
+        <v>4867</v>
       </c>
       <c r="B65" s="0">
         <v>0</v>
@@ -15020,13 +16190,13 @@
         <v>0</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E65" s="0"/>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>4491</v>
+        <v>4868</v>
       </c>
       <c r="B66" s="0">
         <v>0</v>
@@ -15035,43 +16205,43 @@
         <v>0</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E66" s="0"/>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>4492</v>
+        <v>4869</v>
       </c>
       <c r="B67" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C67" s="0">
         <v>0</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E67" s="0"/>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>4493</v>
+        <v>4870</v>
       </c>
       <c r="B68" s="0">
-        <v>0.20000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C68" s="0">
         <v>0</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E68" s="0"/>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>4494</v>
+        <v>4871</v>
       </c>
       <c r="B69" s="0">
         <v>0</v>
@@ -15080,461 +16250,465 @@
         <v>0</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E69" s="0"/>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>4495</v>
+        <v>4872</v>
       </c>
       <c r="B70" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="0">
         <v>0</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E70" s="0"/>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>4496</v>
+        <v>4873</v>
       </c>
       <c r="B71" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C71" s="0">
         <v>0</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E71" s="0"/>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>4497</v>
+        <v>4874</v>
       </c>
       <c r="B72" s="0">
-        <v>0.01</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C72" s="0">
         <v>0</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>4498</v>
+        <v>4875</v>
       </c>
       <c r="B73" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C73" s="0">
         <v>0</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E73" s="0"/>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>4499</v>
+        <v>4876</v>
       </c>
       <c r="B74" s="0">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C74" s="0">
         <v>0</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E74" s="0"/>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>4500</v>
+        <v>4877</v>
       </c>
       <c r="B75" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" s="0">
         <v>0</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E75" s="0"/>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>4501</v>
+        <v>4878</v>
       </c>
       <c r="B76" s="0">
-        <v>0.20000000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="C76" s="0">
         <v>0</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E76" s="0"/>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>4502</v>
+        <v>4879</v>
       </c>
       <c r="B77" s="0">
-        <v>0.94999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="C77" s="0">
         <v>0</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E77" s="0"/>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>4503</v>
+        <v>4880</v>
       </c>
       <c r="B78" s="0">
-        <v>0.90000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="C78" s="0">
         <v>0</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E78" s="0"/>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>4504</v>
+        <v>4881</v>
       </c>
       <c r="B79" s="0">
-        <v>0.14999999999999999</v>
+        <v>1</v>
       </c>
       <c r="C79" s="0">
         <v>0</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E79" s="0"/>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>4505</v>
+        <v>4882</v>
       </c>
       <c r="B80" s="0">
-        <v>0.33333333333333331</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C80" s="0">
         <v>0</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E80" s="0"/>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>4506</v>
+        <v>4883</v>
       </c>
       <c r="B81" s="0">
-        <v>0.69999999999999996</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="C81" s="0">
         <v>0</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>4507</v>
+        <v>4884</v>
       </c>
       <c r="B82" s="0">
-        <v>0.40000000000000002</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="C82" s="0">
         <v>0</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>4508</v>
+        <v>4885</v>
       </c>
       <c r="B83" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="C83" s="0">
         <v>0</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>4509</v>
+        <v>4886</v>
       </c>
       <c r="B84" s="0">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C84" s="0">
         <v>0</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>4510</v>
+        <v>4887</v>
       </c>
       <c r="B85" s="0">
-        <v>0.40000000000000002</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="C85" s="0">
         <v>0</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>4511</v>
+        <v>4888</v>
       </c>
       <c r="B86" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C86" s="0">
         <v>0</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>4512</v>
+        <v>4889</v>
       </c>
       <c r="B87" s="0">
-        <v>0.5</v>
+        <v>0.050000000000000003</v>
       </c>
       <c r="C87" s="0">
         <v>0</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>4513</v>
+        <v>4890</v>
       </c>
       <c r="B88" s="0">
-        <v>1</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="C88" s="0">
         <v>0</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>4514</v>
+        <v>4891</v>
       </c>
       <c r="B89" s="0">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="C89" s="0">
         <v>0</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>4515</v>
+        <v>4892</v>
       </c>
       <c r="B90" s="0">
-        <v>25</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C90" s="0">
         <v>0</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>4516</v>
+        <v>4893</v>
       </c>
       <c r="B91" s="0">
-        <v>1.1000000000000001</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="C91" s="0">
         <v>0</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>4517</v>
+        <v>4894</v>
       </c>
       <c r="B92" s="0">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C92" s="0">
         <v>0</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E92" s="0"/>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>4518</v>
+        <v>4895</v>
       </c>
       <c r="B93" s="0">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C93" s="0">
         <v>0</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E93" s="0"/>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>4519</v>
+        <v>4896</v>
       </c>
       <c r="B94" s="0">
-        <v>3</v>
+        <v>1.01</v>
       </c>
       <c r="C94" s="0">
         <v>0</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E94" s="0"/>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>4520</v>
+        <v>4897</v>
       </c>
       <c r="B95" s="0">
-        <v>0.5</v>
+        <v>25</v>
       </c>
       <c r="C95" s="0">
         <v>0</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E95" s="0"/>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>4521</v>
+        <v>4898</v>
       </c>
       <c r="B96" s="0">
-        <v>4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C96" s="0">
         <v>0</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E96" s="0"/>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>4522</v>
+        <v>4899</v>
       </c>
       <c r="B97" s="0">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C97" s="0">
         <v>0</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E97" s="0"/>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>4523</v>
+        <v>4900</v>
       </c>
       <c r="B98" s="0">
-        <v>0.40000000000000002</v>
+        <v>3</v>
       </c>
       <c r="C98" s="0">
         <v>0</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E98" s="0"/>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>4524</v>
-      </c>
-      <c r="B99" s="0"/>
+        <v>4901</v>
+      </c>
+      <c r="B99" s="0">
+        <v>1.3</v>
+      </c>
       <c r="C99" s="0">
         <v>0</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E99" s="0"/>
+        <v>4932</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>4988</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>4525</v>
+        <v>4902</v>
       </c>
       <c r="B100" s="0">
         <v>0.5</v>
@@ -15543,265 +16717,261 @@
         <v>0</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E100" s="0"/>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>4526</v>
+        <v>4903</v>
       </c>
       <c r="B101" s="0">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="C101" s="0">
         <v>0</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E101" s="0"/>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>4527</v>
+        <v>4904</v>
       </c>
       <c r="B102" s="0">
-        <v>0.40000000000000002</v>
+        <v>2</v>
       </c>
       <c r="C102" s="0">
         <v>0</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E102" s="0"/>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>4528</v>
+        <v>4905</v>
       </c>
       <c r="B103" s="0">
-        <v>0.20000000000000001</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C103" s="0">
         <v>0</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E103" s="0"/>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>4529</v>
+        <v>4906</v>
       </c>
       <c r="B104" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C104" s="0">
         <v>0</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E104" s="0"/>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>4530</v>
+        <v>4907</v>
       </c>
       <c r="B105" s="0">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="C105" s="0">
         <v>0</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E105" s="0"/>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>4531</v>
+        <v>4908</v>
       </c>
       <c r="B106" s="0">
-        <v>0.5</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C106" s="0">
         <v>0</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>4532</v>
+        <v>4909</v>
       </c>
       <c r="B107" s="0">
-        <v>0.5</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C107" s="0">
         <v>0</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E107" s="0"/>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>4533</v>
+        <v>4910</v>
       </c>
       <c r="B108" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C108" s="0">
         <v>0</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E108" s="0"/>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>4534</v>
+        <v>4911</v>
       </c>
       <c r="B109" s="0">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C109" s="0">
         <v>0</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>4603</v>
-      </c>
+        <v>4932</v>
+      </c>
+      <c r="E109" s="0"/>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>4535</v>
+        <v>4912</v>
       </c>
       <c r="B110" s="0">
-        <v>0.69999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="C110" s="0">
         <v>0</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E110" s="0" t="s">
-        <v>4604</v>
-      </c>
+        <v>4932</v>
+      </c>
+      <c r="E110" s="0"/>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>4536</v>
+        <v>4913</v>
       </c>
       <c r="B111" s="0">
-        <v>0.69999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="C111" s="0">
         <v>0</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>4605</v>
-      </c>
+        <v>4932</v>
+      </c>
+      <c r="E111" s="0"/>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>4537</v>
+        <v>4914</v>
       </c>
       <c r="B112" s="0">
-        <v>0.90000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="C112" s="0">
         <v>0</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>4606</v>
-      </c>
+        <v>4932</v>
+      </c>
+      <c r="E112" s="0"/>
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>4538</v>
+        <v>4915</v>
       </c>
       <c r="B113" s="0">
-        <v>0.90000000000000002</v>
+        <v>1</v>
       </c>
       <c r="C113" s="0">
         <v>0</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>4607</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>4539</v>
+        <v>4916</v>
       </c>
       <c r="B114" s="0">
-        <v>0.5</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="C114" s="0">
         <v>0</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>4551</v>
+        <v>4932</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>4608</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>4540</v>
+        <v>4917</v>
       </c>
       <c r="B115" s="0">
-        <v>0.5</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="C115" s="0">
         <v>0</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E115" s="0"/>
+        <v>4932</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>4991</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>4541</v>
+        <v>4918</v>
       </c>
       <c r="B116" s="0">
-        <v>1.02</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="C116" s="0">
         <v>0</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E116" s="0"/>
+        <v>4932</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>4992</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>4542</v>
+        <v>4919</v>
       </c>
       <c r="B117" s="0">
         <v>0.90000000000000002</v>
@@ -15810,40 +16980,104 @@
         <v>0</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E117" s="0"/>
+        <v>4932</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>4993</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>4543</v>
+        <v>4920</v>
       </c>
       <c r="B118" s="0">
-        <v>1.01</v>
+        <v>0.5</v>
       </c>
       <c r="C118" s="0">
         <v>0</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E118" s="0"/>
+        <v>4932</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>4994</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>4544</v>
+        <v>4921</v>
       </c>
       <c r="B119" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="C119" s="0">
         <v>0</v>
       </c>
-      <c r="C119" s="0">
+      <c r="D119" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E119" s="0"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>4922</v>
+      </c>
+      <c r="B120" s="0">
+        <v>1.02</v>
+      </c>
+      <c r="C120" s="0">
+        <v>0</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E120" s="0"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>4923</v>
+      </c>
+      <c r="B121" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="C121" s="0">
+        <v>0</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E121" s="0"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>4924</v>
+      </c>
+      <c r="B122" s="0">
+        <v>1.01</v>
+      </c>
+      <c r="C122" s="0">
+        <v>0</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E122" s="0"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>4925</v>
+      </c>
+      <c r="B123" s="0">
+        <v>0</v>
+      </c>
+      <c r="C123" s="0">
         <v>1</v>
       </c>
-      <c r="D119" s="0" t="s">
-        <v>4551</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>4609</v>
+      <c r="D123" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>4995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>